<commit_message>
Pulping machines + SAM Roasting
</commit_message>
<xml_diff>
--- a/kenya_sut/optimization/ Pulping Machine.xlsx
+++ b/kenya_sut/optimization/ Pulping Machine.xlsx
@@ -540,25 +540,25 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>-0.159999986179173</v>
+        <v>201.6439274931327</v>
       </c>
       <c r="H4">
-        <v>-1</v>
+        <v>1.586955667810023</v>
       </c>
       <c r="I4">
-        <v>-0.0007089301507221535</v>
+        <v>1109.995995204532</v>
       </c>
       <c r="J4">
-        <v>-0.0003299660711491015</v>
+        <v>0.1541644854914921</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0.0007089301507221535</v>
+        <v>1.417860270521487</v>
       </c>
       <c r="M4">
-        <v>0.0003299660711491015</v>
+        <v>0.6599321410685661</v>
       </c>
       <c r="N4">
         <v>0</v>

</xml_diff>